<commit_message>
Research getting data from yr.no
</commit_message>
<xml_diff>
--- a/sample_excel.xlsx
+++ b/sample_excel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="155">
   <si>
     <t>Datums \ Laiks</t>
   </si>
@@ -528,6 +528,18 @@
   </si>
   <si>
     <t>Zīlāni</t>
+  </si>
+  <si>
+    <t>yr.no</t>
+  </si>
+  <si>
+    <t>t min</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>videscentrs.lvgmc.lv</t>
   </si>
 </sst>
 </file>
@@ -1148,16 +1160,16 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -23141,26 +23153,24 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L3:M12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="9">
+        <item x="0"/>
         <item x="1"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="0"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="6"/>
-        <item x="5"/>
+        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -23198,7 +23208,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Average of Sum of summa mm" fld="2" subtotal="average" baseField="0" baseItem="3"/>
   </dataFields>
   <formats count="2">
     <format dxfId="5">
@@ -24091,6 +24101,142 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="28">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="27">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -24149,10 +24295,10 @@
     <dataField name="Average of Sum of kopā mm" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="7">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -24168,7 +24314,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="D1:F37" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="28">
@@ -24548,221 +24694,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="28">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
-        <item x="1"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="27">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="9">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L3:M12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Sum of summa mm" fld="2" subtotal="average" baseField="0" baseItem="3"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="D3:F39" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="5">
@@ -24970,6 +24902,86 @@
     <dataField name="Sum of summa mm" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="2">
     <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
@@ -24980,7 +24992,7 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16/>
@@ -63780,13 +63792,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M353"/>
+  <dimension ref="A1:N353"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63797,12 +63809,18 @@
     <col min="6" max="6" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -63827,8 +63845,17 @@
       <c r="H2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -63847,7 +63874,7 @@
       <c r="F3" s="66"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:B4" si="0">A3</f>
         <v>RV</v>
@@ -63868,7 +63895,7 @@
       <c r="F4" s="66"/>
       <c r="H4" s="48"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" ref="A5:B5" si="3">A4</f>
         <v>RV</v>
@@ -63889,7 +63916,7 @@
       <c r="F5" s="66"/>
       <c r="H5" s="48"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" ref="A6:B6" si="6">A5</f>
         <v>RV</v>
@@ -63910,7 +63937,7 @@
       <c r="F6" s="66"/>
       <c r="H6" s="48"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" ref="A7:B7" si="7">A6</f>
         <v>RV</v>
@@ -63931,7 +63958,7 @@
       <c r="F7" s="66"/>
       <c r="H7" s="48"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" ref="A8:B8" si="8">A7</f>
         <v>RV</v>
@@ -63952,7 +63979,7 @@
       <c r="F8" s="66"/>
       <c r="H8" s="48"/>
     </row>
-    <row r="9" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" ref="A9:B9" si="9">A8</f>
         <v>RV</v>
@@ -63973,7 +64000,7 @@
       <c r="F9" s="66"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" ref="A10:B10" si="10">A9</f>
         <v>RV</v>
@@ -63994,7 +64021,7 @@
       <c r="F10" s="66"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" ref="A11:B11" si="11">A10</f>
         <v>RV</v>
@@ -64015,7 +64042,7 @@
       <c r="F11" s="66"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" ref="A12:B12" si="12">A11</f>
         <v>RV</v>
@@ -64035,7 +64062,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="66"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -64061,7 +64088,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" ref="A14:B16" si="13">A13</f>
         <v>AV</v>
@@ -64089,7 +64116,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="13"/>
         <v>AV</v>
@@ -64117,7 +64144,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="13"/>
         <v>AV</v>

</xml_diff>

<commit_message>
added forecast from yr
</commit_message>
<xml_diff>
--- a/sample_excel.xlsx
+++ b/sample_excel.xlsx
@@ -28,12 +28,12 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="2" r:id="rId11"/>
-    <pivotCache cacheId="3" r:id="rId12"/>
-    <pivotCache cacheId="4" r:id="rId13"/>
-    <pivotCache cacheId="5" r:id="rId14"/>
+    <pivotCache cacheId="6" r:id="rId9"/>
+    <pivotCache cacheId="7" r:id="rId10"/>
+    <pivotCache cacheId="8" r:id="rId11"/>
+    <pivotCache cacheId="9" r:id="rId12"/>
+    <pivotCache cacheId="10" r:id="rId13"/>
+    <pivotCache cacheId="11" r:id="rId14"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="153">
   <si>
     <t>Datums \ Laiks</t>
   </si>
@@ -533,12 +533,6 @@
     <t>yr.no</t>
   </si>
   <si>
-    <t>t min</t>
-  </si>
-  <si>
-    <t>avg</t>
-  </si>
-  <si>
     <t>videscentrs.lvgmc.lv</t>
   </si>
 </sst>
@@ -922,7 +916,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,6 +1100,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1160,40 +1155,13 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -1275,6 +1243,33 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -22875,363 +22870,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A2:W11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="28">
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="9">
-        <item h="1" x="5"/>
-        <item x="1"/>
-        <item h="1" x="3"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="7"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="27">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="25">
-        <item m="1" x="14"/>
-        <item m="1" x="21"/>
-        <item m="1" x="8"/>
-        <item m="1" x="15"/>
-        <item m="1" x="23"/>
-        <item m="1" x="13"/>
-        <item m="1" x="22"/>
-        <item m="1" x="19"/>
-        <item m="1" x="11"/>
-        <item m="1" x="20"/>
-        <item m="1" x="12"/>
-        <item m="1" x="16"/>
-        <item m="1" x="7"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item m="1" x="18"/>
-        <item m="1" x="10"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="0"/>
-    <field x="1"/>
-  </colFields>
-  <colItems count="22">
-    <i>
-      <x v="1"/>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="25"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="9">
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="17">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="16">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="15">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
-    </format>
-    <format dxfId="14">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="11">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-          <reference field="1" count="5">
-            <x v="8"/>
-            <x v="9"/>
-            <x v="12"/>
-            <x v="22"/>
-            <x v="23"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="4">
-            <x v="4"/>
-            <x v="5"/>
-            <x v="17"/>
-            <x v="25"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L3:M12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Sum of summa mm" fld="2" subtotal="average" baseField="0" baseItem="3"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="5">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A22:W34" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
@@ -23441,32 +23080,32 @@
     <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="4" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="27">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="16">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="15">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="14">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -23481,7 +23120,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -23510,8 +23149,86 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L3:M12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Sum of summa mm" fld="2" subtotal="average" baseField="0" baseItem="3"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A35:W47" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
@@ -23766,32 +23483,32 @@
     <dataField name="Average of summa mm" fld="3" subtotal="average" baseField="4" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="36">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="25">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="24">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="23">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -23806,7 +23523,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -23835,8 +23552,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A12:W21" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="28">
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
@@ -24034,29 +23751,29 @@
     <dataField name="Average of kopā mm" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="44">
+    <format dxfId="35">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="34">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="33">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="32">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -24071,7 +23788,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -24100,30 +23817,30 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A2:W11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="28">
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="9">
+        <item h="1" x="5"/>
         <item x="1"/>
-        <item x="7"/>
+        <item h="1" x="3"/>
         <item x="4"/>
+        <item x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="7"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="27">
         <item x="0"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="27">
-        <item x="0"/>
+        <item x="4"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
@@ -24148,80 +23865,222 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="25">
+        <item m="1" x="14"/>
+        <item m="1" x="21"/>
+        <item m="1" x="8"/>
+        <item m="1" x="15"/>
+        <item m="1" x="23"/>
+        <item m="1" x="13"/>
+        <item m="1" x="22"/>
+        <item m="1" x="19"/>
+        <item m="1" x="11"/>
+        <item m="1" x="20"/>
+        <item m="1" x="12"/>
+        <item m="1" x="16"/>
+        <item m="1" x="7"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item m="1" x="18"/>
+        <item m="1" x="10"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="0"/>
+    <field x="3"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="7">
     <i>
-      <x/>
+      <x v="17"/>
     </i>
     <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="22">
+    <i>
+      <x v="1"/>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i t="default">
       <x v="1"/>
     </i>
     <i>
+      <x v="3"/>
       <x v="2"/>
     </i>
-    <i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i t="default">
       <x v="3"/>
     </i>
     <i>
       <x v="4"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
     </i>
     <i>
-      <x v="5"/>
+      <x v="7"/>
+      <x v="8"/>
     </i>
-    <i>
-      <x v="6"/>
+    <i r="1">
+      <x v="9"/>
     </i>
-    <i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i t="default">
       <x v="7"/>
     </i>
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
-    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <formats count="2">
-    <format dxfId="7">
+  <formats count="9">
+    <format dxfId="44">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="43">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    <format dxfId="42">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="41">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="39">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="1" count="5">
+            <x v="8"/>
+            <x v="9"/>
+            <x v="12"/>
+            <x v="22"/>
+            <x v="23"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="4">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="17"/>
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -24230,14 +24089,14 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -24295,10 +24154,10 @@
     <dataField name="Average of Sum of kopā mm" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="9">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -24314,8 +24173,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="D1:F37" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="28">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -24694,8 +24553,144 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="28">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="27">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of Vidējā t" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="9">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="D3:F39" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -24922,7 +24917,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -25317,32 +25312,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="129" t="s">
+      <c r="B1" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="129"/>
-      <c r="D1" s="131" t="s">
+      <c r="C1" s="130"/>
+      <c r="D1" s="132" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="132"/>
-      <c r="F1" s="133" t="s">
+      <c r="E1" s="133"/>
+      <c r="F1" s="134" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133" t="s">
+      <c r="G1" s="134"/>
+      <c r="H1" s="134" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="133"/>
-      <c r="J1" s="127" t="s">
+      <c r="I1" s="134"/>
+      <c r="J1" s="128" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="128"/>
+      <c r="K1" s="129"/>
     </row>
     <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="130"/>
+      <c r="A2" s="131"/>
       <c r="B2" s="18" t="s">
         <v>80</v>
       </c>
@@ -26358,26 +26353,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134" t="s">
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134" t="s">
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134" t="s">
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="134"/>
-      <c r="O1" s="134"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
       <c r="P1" s="40" t="s">
         <v>96</v>
       </c>
@@ -34018,31 +34013,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="135"/>
-      <c r="U1" s="135"/>
-      <c r="V1" s="135"/>
-      <c r="W1" s="135"/>
-      <c r="X1" s="135"/>
-      <c r="Y1" s="135"/>
-      <c r="Z1" s="135"/>
-      <c r="AA1" s="135"/>
-      <c r="AB1" s="135"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136"/>
+      <c r="S1" s="136"/>
+      <c r="T1" s="136"/>
+      <c r="U1" s="136"/>
+      <c r="V1" s="136"/>
+      <c r="W1" s="136"/>
+      <c r="X1" s="136"/>
+      <c r="Y1" s="136"/>
+      <c r="Z1" s="136"/>
+      <c r="AA1" s="136"/>
+      <c r="AB1" s="136"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -48924,31 +48919,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="135"/>
-      <c r="U1" s="135"/>
-      <c r="V1" s="135"/>
-      <c r="W1" s="135"/>
-      <c r="X1" s="135"/>
-      <c r="Y1" s="135"/>
-      <c r="Z1" s="135"/>
-      <c r="AA1" s="135"/>
-      <c r="AB1" s="135"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
+      <c r="Q1" s="136"/>
+      <c r="R1" s="136"/>
+      <c r="S1" s="136"/>
+      <c r="T1" s="136"/>
+      <c r="U1" s="136"/>
+      <c r="V1" s="136"/>
+      <c r="W1" s="136"/>
+      <c r="X1" s="136"/>
+      <c r="Y1" s="136"/>
+      <c r="Z1" s="136"/>
+      <c r="AA1" s="136"/>
+      <c r="AB1" s="136"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -63792,13 +63787,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N353"/>
+  <dimension ref="A1:M353"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63809,18 +63804,18 @@
     <col min="6" max="6" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="14" t="s">
         <v>106</v>
       </c>
       <c r="J1" t="s">
         <v>151</v>
       </c>
-      <c r="N1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -63845,17 +63840,14 @@
       <c r="H2" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" t="s">
-        <v>152</v>
-      </c>
-      <c r="L2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="127" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -63874,7 +63866,7 @@
       <c r="F3" s="66"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:B4" si="0">A3</f>
         <v>RV</v>
@@ -63895,7 +63887,7 @@
       <c r="F4" s="66"/>
       <c r="H4" s="48"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f t="shared" ref="A5:B5" si="3">A4</f>
         <v>RV</v>
@@ -63916,7 +63908,7 @@
       <c r="F5" s="66"/>
       <c r="H5" s="48"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
         <f t="shared" ref="A6:B6" si="6">A5</f>
         <v>RV</v>
@@ -63937,7 +63929,7 @@
       <c r="F6" s="66"/>
       <c r="H6" s="48"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
         <f t="shared" ref="A7:B7" si="7">A6</f>
         <v>RV</v>
@@ -63958,7 +63950,7 @@
       <c r="F7" s="66"/>
       <c r="H7" s="48"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
         <f t="shared" ref="A8:B8" si="8">A7</f>
         <v>RV</v>
@@ -63979,7 +63971,7 @@
       <c r="F8" s="66"/>
       <c r="H8" s="48"/>
     </row>
-    <row r="9" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
         <f t="shared" ref="A9:B9" si="9">A8</f>
         <v>RV</v>
@@ -64000,7 +63992,7 @@
       <c r="F9" s="66"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
         <f t="shared" ref="A10:B10" si="10">A9</f>
         <v>RV</v>
@@ -64021,7 +64013,7 @@
       <c r="F10" s="66"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
         <f t="shared" ref="A11:B11" si="11">A10</f>
         <v>RV</v>
@@ -64042,7 +64034,7 @@
       <c r="F11" s="66"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
         <f t="shared" ref="A12:B12" si="12">A11</f>
         <v>RV</v>
@@ -64062,7 +64054,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="66"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -64088,7 +64080,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
         <f t="shared" ref="A14:B16" si="13">A13</f>
         <v>AV</v>
@@ -64116,7 +64108,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
         <f t="shared" si="13"/>
         <v>AV</v>
@@ -64144,7 +64136,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f t="shared" si="13"/>
         <v>AV</v>

</xml_diff>